<commit_message>
prep for test 4
</commit_message>
<xml_diff>
--- a/final_results.xlsx
+++ b/final_results.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" tabRatio="598"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" tabRatio="598" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="1" r:id="rId1"/>
     <sheet name="test1" sheetId="2" r:id="rId2"/>
     <sheet name="test2" sheetId="3" r:id="rId3"/>
     <sheet name="test3" sheetId="4" r:id="rId4"/>
+    <sheet name="test4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="26">
   <si>
     <t>My Template Matching</t>
   </si>
@@ -90,12 +91,18 @@
   <si>
     <t>Feature (keypoint) Matching</t>
   </si>
+  <si>
+    <t>Synthetic test data</t>
+  </si>
+  <si>
+    <t>Real test data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +132,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -244,7 +259,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,6 +292,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -582,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I8"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -595,6 +619,14 @@
     <col min="6" max="16384" width="31.42578125" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>3</v>
@@ -743,7 +775,71 @@
         <v>11</v>
       </c>
     </row>
+    <row r="9" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5307,8 +5403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ33"/>
   <sheetViews>
-    <sheetView topLeftCell="AF10" workbookViewId="0">
-      <selection activeCell="AN32" sqref="AN32"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7564,4 +7660,248 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="18.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
advanced alg test results
</commit_message>
<xml_diff>
--- a/final_results.xlsx
+++ b/final_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" tabRatio="598"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" tabRatio="598" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="test2" sheetId="3" r:id="rId3"/>
     <sheet name="test3" sheetId="4" r:id="rId4"/>
     <sheet name="test4" sheetId="5" r:id="rId5"/>
+    <sheet name="test5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="27">
   <si>
     <t>My Template Matching</t>
   </si>
@@ -94,12 +95,18 @@
   <si>
     <t>Real test data</t>
   </si>
+  <si>
+    <t>Advanced Template Matching</t>
+  </si>
+  <si>
+    <t>Feature Matching replaced with Advanced Template Matching (My Template Matching + Multi-Scale Template Matching)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,8 +150,24 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,8 +221,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -250,13 +278,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -294,17 +338,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Вывод" xfId="1" builtinId="21"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Пояснение" xfId="2" builtinId="53"/>
+    <cellStyle name="Примечание" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -603,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -617,12 +668,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -779,12 +830,12 @@
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10"/>
@@ -850,10 +901,247 @@
       <c r="H13"/>
       <c r="I13"/>
     </row>
+    <row r="15" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="17" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2">
+        <f>test1!AO53</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <f>test1!AP53</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <f>test1!AQ53</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <f>test1!AO54</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <f>test1!AP54</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="10">
+        <f>test1!AQ54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2">
+        <f>test2!AO53</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <f>test2!AP53</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <f>test2!AQ53</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="2">
+        <f>test2!AO54</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <f>test2!AP54</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <f>test2!AQ54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2">
+        <f>test3!AO53</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <f>test3!AP53</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <f>test3!AQ53</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <f>test3!AO54</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="10">
+        <f>test3!AP54</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <f>test3!AQ54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="4">
+        <f>test5!U38</f>
+        <v>0.71581422734065803</v>
+      </c>
+      <c r="C28" s="2">
+        <f>test5!V38</f>
+        <v>0.77307060498150704</v>
+      </c>
+      <c r="D28" s="10">
+        <f>test5!W38</f>
+        <v>0.71728736646813007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2">
+        <f>test5!U39</f>
+        <v>3.5032950040961922E-3</v>
+      </c>
+      <c r="C29" s="4">
+        <f>test5!V39</f>
+        <v>1.8794900002346064E-2</v>
+      </c>
+      <c r="D29" s="10">
+        <f>test5!W39</f>
+        <v>1.7623480006780788E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7681,8 +7969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView topLeftCell="L10" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T32" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9168,7 +9456,7 @@
         <v>0.93069458845431086</v>
       </c>
       <c r="B38" s="6">
-        <f t="shared" ref="B38:D39" si="0">AVERAGE(B2,B5,B8,B11,B14,B17,B20,B23,B26,B29,B32,B35)</f>
+        <f t="shared" ref="B38:C39" si="0">AVERAGE(B2,B5,B8,B11,B14,B17,B20,B23,B26,B29,B32,B35)</f>
         <v>0.93069458845431086</v>
       </c>
       <c r="C38" s="6">
@@ -9321,4 +9609,1642 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="18.42578125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.92014042937500751</v>
+      </c>
+      <c r="B2">
+        <v>0.92014042937500751</v>
+      </c>
+      <c r="C2">
+        <v>0.92014042937500751</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="F2">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="G2">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="J2">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="K2">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="L2"/>
+      <c r="M2">
+        <v>0.62517221585294003</v>
+      </c>
+      <c r="N2">
+        <v>0.62517221585294003</v>
+      </c>
+      <c r="O2">
+        <v>0.62517221585294003</v>
+      </c>
+      <c r="P2"/>
+      <c r="Q2">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="R2">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="S2">
+        <v>0.89473684210526316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.750600000377744E-3</v>
+      </c>
+      <c r="B3">
+        <v>6.772099994122982E-3</v>
+      </c>
+      <c r="C3">
+        <v>5.2465000189840794E-3</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3">
+        <v>4.1006000246852636E-3</v>
+      </c>
+      <c r="F3">
+        <v>1.8729300005361441E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.9788600038737059E-2</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3">
+        <v>1.0092300013639029E-2</v>
+      </c>
+      <c r="J3">
+        <v>2.6965499971993271E-2</v>
+      </c>
+      <c r="K3">
+        <v>2.240869996603578E-2</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3">
+        <v>5.6254999944940209E-3</v>
+      </c>
+      <c r="N3">
+        <v>3.0283300031442199E-2</v>
+      </c>
+      <c r="O3">
+        <v>3.1321899965405457E-2</v>
+      </c>
+      <c r="P3"/>
+      <c r="Q3">
+        <v>2.321399981155992E-3</v>
+      </c>
+      <c r="R3">
+        <v>1.8039400049019601E-2</v>
+      </c>
+      <c r="S3">
+        <v>1.840840000659227E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.92014042937500751</v>
+      </c>
+      <c r="B5">
+        <v>0.92014042937500751</v>
+      </c>
+      <c r="C5">
+        <v>0.92014042937500751</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="F5">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="G5">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5">
+        <v>0.70005767567101262</v>
+      </c>
+      <c r="J5">
+        <v>0.70005767567101262</v>
+      </c>
+      <c r="K5">
+        <v>0.70005767567101262</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5">
+        <v>0.35717565346677488</v>
+      </c>
+      <c r="N5">
+        <v>0.35717565346677488</v>
+      </c>
+      <c r="O5">
+        <v>0.35717565346677488</v>
+      </c>
+      <c r="P5"/>
+      <c r="Q5">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="R5">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="S5">
+        <v>0.89473684210526316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7.0319999940693378E-4</v>
+      </c>
+      <c r="B6">
+        <v>5.6864999933168292E-3</v>
+      </c>
+      <c r="C6">
+        <v>1.289280003402382E-2</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6">
+        <v>4.0598999476060271E-3</v>
+      </c>
+      <c r="F6">
+        <v>2.2815399977844208E-2</v>
+      </c>
+      <c r="G6">
+        <v>2.175389998592436E-2</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6">
+        <v>5.0912000006064773E-3</v>
+      </c>
+      <c r="J6">
+        <v>1.9293699995614592E-2</v>
+      </c>
+      <c r="K6">
+        <v>1.5471699996851379E-2</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6">
+        <v>6.293600017670542E-3</v>
+      </c>
+      <c r="N6">
+        <v>3.7513700022827827E-2</v>
+      </c>
+      <c r="O6">
+        <v>2.9515700007323179E-2</v>
+      </c>
+      <c r="P6"/>
+      <c r="Q6">
+        <v>3.2242000452242792E-3</v>
+      </c>
+      <c r="R6">
+        <v>1.963220001198351E-2</v>
+      </c>
+      <c r="S6">
+        <v>1.8767800007481131E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.85714285714285721</v>
+      </c>
+      <c r="B8">
+        <v>0.85714285714285721</v>
+      </c>
+      <c r="C8">
+        <v>0.85714285714285721</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8">
+        <v>0.9168109669192297</v>
+      </c>
+      <c r="F8">
+        <v>0.9168109669192297</v>
+      </c>
+      <c r="G8">
+        <v>0.9168109669192297</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="J8">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="K8">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="N8">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="O8">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="P8"/>
+      <c r="Q8">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="R8">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="S8">
+        <v>0.88231221171053742</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7.0570001844316721E-4</v>
+      </c>
+      <c r="B9">
+        <v>5.2011000225320458E-3</v>
+      </c>
+      <c r="C9">
+        <v>5.4754000157117844E-3</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9">
+        <v>5.3711999789811671E-3</v>
+      </c>
+      <c r="F9">
+        <v>4.2590700031723827E-2</v>
+      </c>
+      <c r="G9">
+        <v>2.8108200000133369E-2</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9">
+        <v>5.8445000322535634E-3</v>
+      </c>
+      <c r="J9">
+        <v>3.3329400001093752E-2</v>
+      </c>
+      <c r="K9">
+        <v>3.1899800000246607E-2</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9">
+        <v>5.9646000154316434E-3</v>
+      </c>
+      <c r="N9">
+        <v>3.3194999967236072E-2</v>
+      </c>
+      <c r="O9">
+        <v>2.8866900014691051E-2</v>
+      </c>
+      <c r="P9"/>
+      <c r="Q9">
+        <v>4.0578999905847013E-3</v>
+      </c>
+      <c r="R9">
+        <v>2.4901000026147809E-2</v>
+      </c>
+      <c r="S9">
+        <v>2.4216099991463121E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.88706151213684359</v>
+      </c>
+      <c r="B11">
+        <v>0.88706151213684359</v>
+      </c>
+      <c r="C11">
+        <v>0.88706151213684359</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="F11">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="G11">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="J11">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="K11">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="N11">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="O11">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="P11"/>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3.7989998236298561E-4</v>
+      </c>
+      <c r="B12">
+        <v>3.1326999887824059E-3</v>
+      </c>
+      <c r="C12">
+        <v>4.0662999963387847E-3</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12">
+        <v>4.5809999573975801E-3</v>
+      </c>
+      <c r="F12">
+        <v>1.294710004003718E-2</v>
+      </c>
+      <c r="G12">
+        <v>1.203859999077395E-2</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12">
+        <v>2.3556000087410212E-3</v>
+      </c>
+      <c r="J12">
+        <v>7.7905000071041286E-3</v>
+      </c>
+      <c r="K12">
+        <v>8.0561000504530966E-3</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12">
+        <v>3.3039000118151311E-3</v>
+      </c>
+      <c r="N12">
+        <v>2.8037699987180531E-2</v>
+      </c>
+      <c r="O12">
+        <v>2.4153799982741479E-2</v>
+      </c>
+      <c r="P12"/>
+      <c r="Q12">
+        <v>1.9466000376269219E-3</v>
+      </c>
+      <c r="R12">
+        <v>1.1104600038379431E-2</v>
+      </c>
+      <c r="S12">
+        <v>1.0167200001887981E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.96551724137931039</v>
+      </c>
+      <c r="B14">
+        <v>0.96551724137931039</v>
+      </c>
+      <c r="C14">
+        <v>0.96551724137931039</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14">
+        <v>0.9375</v>
+      </c>
+      <c r="F14">
+        <v>0.9375</v>
+      </c>
+      <c r="G14">
+        <v>0.9375</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14">
+        <v>0.8125</v>
+      </c>
+      <c r="J14">
+        <v>0.8125</v>
+      </c>
+      <c r="K14">
+        <v>0.8125</v>
+      </c>
+      <c r="L14"/>
+      <c r="M14">
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="N14">
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="O14">
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="P14"/>
+      <c r="Q14">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="R14">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="S14">
+        <v>0.89473684210526316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5.8890000218525529E-4</v>
+      </c>
+      <c r="B15">
+        <v>4.5496000093407929E-3</v>
+      </c>
+      <c r="C15">
+        <v>5.2354999934323132E-3</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15">
+        <v>2.410699962638319E-3</v>
+      </c>
+      <c r="F15">
+        <v>1.869340002303943E-2</v>
+      </c>
+      <c r="G15">
+        <v>1.234650000697002E-2</v>
+      </c>
+      <c r="H15"/>
+      <c r="I15">
+        <v>5.7208999642170966E-3</v>
+      </c>
+      <c r="J15">
+        <v>2.294270001584664E-2</v>
+      </c>
+      <c r="K15">
+        <v>2.7011100028175861E-2</v>
+      </c>
+      <c r="L15"/>
+      <c r="M15">
+        <v>3.5222000442445278E-3</v>
+      </c>
+      <c r="N15">
+        <v>3.1156399985775352E-2</v>
+      </c>
+      <c r="O15">
+        <v>3.012310003396124E-2</v>
+      </c>
+      <c r="P15"/>
+      <c r="Q15">
+        <v>3.21659998735413E-3</v>
+      </c>
+      <c r="R15">
+        <v>1.7013599979691211E-2</v>
+      </c>
+      <c r="S15">
+        <v>1.4948800031561399E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.92289420767242103</v>
+      </c>
+      <c r="B17">
+        <v>0.92289420767242103</v>
+      </c>
+      <c r="C17">
+        <v>0.92289420767242103</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17">
+        <v>0.9375</v>
+      </c>
+      <c r="F17">
+        <v>0.9375</v>
+      </c>
+      <c r="G17">
+        <v>0.9375</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17">
+        <v>0.74230589839889616</v>
+      </c>
+      <c r="J17">
+        <v>0.74230589839889616</v>
+      </c>
+      <c r="K17">
+        <v>0.74230589839889616</v>
+      </c>
+      <c r="L17"/>
+      <c r="M17">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="N17">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="O17">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="P17"/>
+      <c r="Q17">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="R17">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="S17">
+        <v>0.89473684210526316</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5.8170000556856394E-4</v>
+      </c>
+      <c r="B18">
+        <v>6.4032000373117626E-3</v>
+      </c>
+      <c r="C18">
+        <v>4.7610999899916351E-3</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18">
+        <v>2.4613999994471669E-3</v>
+      </c>
+      <c r="F18">
+        <v>1.8202400009613481E-2</v>
+      </c>
+      <c r="G18">
+        <v>1.768739998806268E-2</v>
+      </c>
+      <c r="H18"/>
+      <c r="I18">
+        <v>5.4495999938808382E-3</v>
+      </c>
+      <c r="J18">
+        <v>1.9394900009501729E-2</v>
+      </c>
+      <c r="K18">
+        <v>2.065789996413514E-2</v>
+      </c>
+      <c r="L18"/>
+      <c r="M18">
+        <v>4.3817000114358962E-3</v>
+      </c>
+      <c r="N18">
+        <v>3.1434000004082918E-2</v>
+      </c>
+      <c r="O18">
+        <v>3.183230001013726E-2</v>
+      </c>
+      <c r="P18"/>
+      <c r="Q18">
+        <v>3.2642000005580481E-3</v>
+      </c>
+      <c r="R18">
+        <v>1.973110000835732E-2</v>
+      </c>
+      <c r="S18">
+        <v>1.9107700034510341E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.95123401509058292</v>
+      </c>
+      <c r="B20">
+        <v>0.95123401509058292</v>
+      </c>
+      <c r="C20">
+        <v>0.95123401509058292</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20">
+        <v>0.82322330470336313</v>
+      </c>
+      <c r="F20">
+        <v>0.91161165235168151</v>
+      </c>
+      <c r="G20">
+        <v>0.91161165235168151</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20">
+        <v>0.80235764623947625</v>
+      </c>
+      <c r="J20">
+        <v>0.80235764623947625</v>
+      </c>
+      <c r="K20">
+        <v>0.80235764623947625</v>
+      </c>
+      <c r="L20"/>
+      <c r="M20">
+        <v>0.15035684483174919</v>
+      </c>
+      <c r="N20">
+        <v>0.15035684483174919</v>
+      </c>
+      <c r="O20">
+        <v>0.15035684483174919</v>
+      </c>
+      <c r="P20"/>
+      <c r="Q20">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="R20">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="S20">
+        <v>0.88231221171053742</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5.9880001936107874E-4</v>
+      </c>
+      <c r="B21">
+        <v>4.8862000112421811E-3</v>
+      </c>
+      <c r="C21">
+        <v>8.8753000018186867E-3</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21">
+        <v>6.1304999981075534E-3</v>
+      </c>
+      <c r="F21">
+        <v>2.6562999992165711E-2</v>
+      </c>
+      <c r="G21">
+        <v>2.1914400043897331E-2</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21">
+        <v>8.7870000279508531E-3</v>
+      </c>
+      <c r="J21">
+        <v>3.4934299997985363E-2</v>
+      </c>
+      <c r="K21">
+        <v>3.361909999512136E-2</v>
+      </c>
+      <c r="L21"/>
+      <c r="M21">
+        <v>5.6852000416256487E-3</v>
+      </c>
+      <c r="N21">
+        <v>2.8534899989608679E-2</v>
+      </c>
+      <c r="O21">
+        <v>2.9242400021757931E-2</v>
+      </c>
+      <c r="P21"/>
+      <c r="Q21">
+        <v>6.210200022906065E-3</v>
+      </c>
+      <c r="R21">
+        <v>2.490419999230653E-2</v>
+      </c>
+      <c r="S21">
+        <v>2.560900000389665E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23">
+        <v>0.9375</v>
+      </c>
+      <c r="F23">
+        <v>0.9375</v>
+      </c>
+      <c r="G23">
+        <v>0.9375</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23">
+        <v>0.8125</v>
+      </c>
+      <c r="J23">
+        <v>0.8125</v>
+      </c>
+      <c r="K23">
+        <v>0.8125</v>
+      </c>
+      <c r="L23"/>
+      <c r="M23">
+        <v>0.15035684483174919</v>
+      </c>
+      <c r="N23">
+        <v>0.15035684483174919</v>
+      </c>
+      <c r="O23">
+        <v>0.15035684483174919</v>
+      </c>
+      <c r="P23"/>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1.204999978654087E-3</v>
+      </c>
+      <c r="B24">
+        <v>4.5399999944493166E-3</v>
+      </c>
+      <c r="C24">
+        <v>3.7256000214256351E-3</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24">
+        <v>8.8090001372620463E-4</v>
+      </c>
+      <c r="F24">
+        <v>1.011239999206737E-2</v>
+      </c>
+      <c r="G24">
+        <v>1.018079998902977E-2</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24">
+        <v>1.4468000154010949E-3</v>
+      </c>
+      <c r="J24">
+        <v>7.9663999495096505E-3</v>
+      </c>
+      <c r="K24">
+        <v>8.1759000313468277E-3</v>
+      </c>
+      <c r="L24"/>
+      <c r="M24">
+        <v>3.5606999881565571E-3</v>
+      </c>
+      <c r="N24">
+        <v>2.2245000000111759E-2</v>
+      </c>
+      <c r="O24">
+        <v>2.0802600018214431E-2</v>
+      </c>
+      <c r="P24"/>
+      <c r="Q24">
+        <v>1.872299995739013E-3</v>
+      </c>
+      <c r="R24">
+        <v>7.695100037381053E-3</v>
+      </c>
+      <c r="S24">
+        <v>5.6150999735109508E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="B26">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="C26">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="F26">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="G26">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="H26"/>
+      <c r="I26">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="J26">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="K26">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="L26"/>
+      <c r="M26">
+        <v>0.68283802879864153</v>
+      </c>
+      <c r="N26">
+        <v>0.68283802879864153</v>
+      </c>
+      <c r="O26">
+        <v>0.68283802879864153</v>
+      </c>
+      <c r="P26"/>
+      <c r="Q26">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="R26">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="S26">
+        <v>0.89473684210526316</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9.4319996424019337E-4</v>
+      </c>
+      <c r="B27">
+        <v>7.0374999777413896E-3</v>
+      </c>
+      <c r="C27">
+        <v>3.7295999936759472E-3</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27">
+        <v>3.544999985024333E-3</v>
+      </c>
+      <c r="F27">
+        <v>1.467540004523471E-2</v>
+      </c>
+      <c r="G27">
+        <v>1.3535999984014779E-2</v>
+      </c>
+      <c r="H27"/>
+      <c r="I27">
+        <v>5.4140000138431787E-3</v>
+      </c>
+      <c r="J27">
+        <v>2.9484200000297282E-2</v>
+      </c>
+      <c r="K27">
+        <v>2.444850001484156E-2</v>
+      </c>
+      <c r="L27"/>
+      <c r="M27">
+        <v>3.655500011518598E-3</v>
+      </c>
+      <c r="N27">
+        <v>3.112170001259074E-2</v>
+      </c>
+      <c r="O27">
+        <v>2.7435199997853491E-2</v>
+      </c>
+      <c r="P27"/>
+      <c r="Q27">
+        <v>3.4096000017598271E-3</v>
+      </c>
+      <c r="R27">
+        <v>1.3748099969234319E-2</v>
+      </c>
+      <c r="S27">
+        <v>1.7285500012803819E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.88706151213684359</v>
+      </c>
+      <c r="B29">
+        <v>0.88706151213684359</v>
+      </c>
+      <c r="C29">
+        <v>0.88706151213684359</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="F29">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="G29">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="H29"/>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0.70005767567101262</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29"/>
+      <c r="M29">
+        <v>0.45607170677957881</v>
+      </c>
+      <c r="N29">
+        <v>0.45607170677957881</v>
+      </c>
+      <c r="O29">
+        <v>0.45607170677957881</v>
+      </c>
+      <c r="P29"/>
+      <c r="Q29">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="R29">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="S29">
+        <v>0.89473684210526316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7.4030004907399416E-4</v>
+      </c>
+      <c r="B30">
+        <v>4.5917999814264476E-3</v>
+      </c>
+      <c r="C30">
+        <v>2.4863000144250691E-3</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30">
+        <v>2.653200004715472E-3</v>
+      </c>
+      <c r="F30">
+        <v>1.554940000642091E-2</v>
+      </c>
+      <c r="G30">
+        <v>1.001750002615154E-2</v>
+      </c>
+      <c r="H30"/>
+      <c r="I30">
+        <v>3.600900003220886E-3</v>
+      </c>
+      <c r="J30">
+        <v>1.945850002812222E-2</v>
+      </c>
+      <c r="K30">
+        <v>1.840400003129616E-2</v>
+      </c>
+      <c r="L30"/>
+      <c r="M30">
+        <v>6.0357000329531729E-3</v>
+      </c>
+      <c r="N30">
+        <v>2.8814599965699021E-2</v>
+      </c>
+      <c r="O30">
+        <v>2.7740499994251881E-2</v>
+      </c>
+      <c r="P30"/>
+      <c r="Q30">
+        <v>3.1539999763481319E-3</v>
+      </c>
+      <c r="R30">
+        <v>1.8574099987745289E-2</v>
+      </c>
+      <c r="S30">
+        <v>1.889300002949312E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="B32">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="C32">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32">
+        <v>0.90571909584179366</v>
+      </c>
+      <c r="F32">
+        <v>0.90571909584179366</v>
+      </c>
+      <c r="G32">
+        <v>0.90571909584179366</v>
+      </c>
+      <c r="H32"/>
+      <c r="I32">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="J32">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="K32">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="L32"/>
+      <c r="M32">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="N32">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="O32">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="P32"/>
+      <c r="Q32">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="R32">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="S32">
+        <v>0.88231221171053742</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1.840299984905869E-3</v>
+      </c>
+      <c r="B33">
+        <v>5.2059000008739531E-3</v>
+      </c>
+      <c r="C33">
+        <v>4.940000013448298E-3</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33">
+        <v>3.6659000325016682E-3</v>
+      </c>
+      <c r="F33">
+        <v>1.9850699987728149E-2</v>
+      </c>
+      <c r="G33">
+        <v>2.0131000026594851E-2</v>
+      </c>
+      <c r="H33"/>
+      <c r="I33">
+        <v>7.7664999989792696E-3</v>
+      </c>
+      <c r="J33">
+        <v>3.9260899997316301E-2</v>
+      </c>
+      <c r="K33">
+        <v>3.3638500026427209E-2</v>
+      </c>
+      <c r="L33"/>
+      <c r="M33">
+        <v>4.8919999971985817E-3</v>
+      </c>
+      <c r="N33">
+        <v>3.0473000020720061E-2</v>
+      </c>
+      <c r="O33">
+        <v>3.2399399962741882E-2</v>
+      </c>
+      <c r="P33"/>
+      <c r="Q33">
+        <v>5.0261999713256964E-3</v>
+      </c>
+      <c r="R33">
+        <v>2.111390000209212E-2</v>
+      </c>
+      <c r="S33">
+        <v>2.548499999102205E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="B35">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="C35">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="F35">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="G35">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="H35"/>
+      <c r="I35">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="J35">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="K35">
+        <v>0.75746437496366703</v>
+      </c>
+      <c r="L35"/>
+      <c r="M35">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="N35">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="O35">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="P35"/>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0.88231221171053742</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5.1749998237937689E-4</v>
+      </c>
+      <c r="B36">
+        <v>6.876500032376498E-3</v>
+      </c>
+      <c r="C36">
+        <v>4.1041999938897789E-3</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36">
+        <v>1.741200045216829E-3</v>
+      </c>
+      <c r="F36">
+        <v>9.4600999727845192E-3</v>
+      </c>
+      <c r="G36">
+        <v>7.4071999988518664E-3</v>
+      </c>
+      <c r="H36"/>
+      <c r="I36">
+        <v>1.00020004902035E-3</v>
+      </c>
+      <c r="J36">
+        <v>8.0794999958015978E-3</v>
+      </c>
+      <c r="K36">
+        <v>7.299999997485429E-3</v>
+      </c>
+      <c r="L36"/>
+      <c r="M36">
+        <v>3.0270999995991592E-3</v>
+      </c>
+      <c r="N36">
+        <v>2.6133699982892718E-2</v>
+      </c>
+      <c r="O36">
+        <v>2.5991700007580221E-2</v>
+      </c>
+      <c r="P36"/>
+      <c r="Q36">
+        <v>1.820700010284781E-3</v>
+      </c>
+      <c r="R36">
+        <v>8.3207999705336988E-3</v>
+      </c>
+      <c r="S36">
+        <v>7.9397000372409821E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <f>AVERAGE(A2,A5,A8,A11,A14,A17,A20,A23,A26,A29,A32,A35)</f>
+        <v>0.93069458845431086</v>
+      </c>
+      <c r="B38" s="6">
+        <f t="shared" ref="B38:C39" si="0">AVERAGE(B2,B5,B8,B11,B14,B17,B20,B23,B26,B29,B32,B35)</f>
+        <v>0.93069458845431086</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="0"/>
+        <v>0.93069458845431086</v>
+      </c>
+      <c r="E38" s="6">
+        <f t="shared" ref="E38:S39" si="1">AVERAGE(E2,E5,E8,E11,E14,E17,E20,E23,E26,E29,E32,E35)</f>
+        <v>0.92348189826909122</v>
+      </c>
+      <c r="F38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.930847593906451</v>
+      </c>
+      <c r="G38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.930847593906451</v>
+      </c>
+      <c r="I38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.70301933268826744</v>
+      </c>
+      <c r="J38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.7613574723275186</v>
+      </c>
+      <c r="K38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.70301933268826744</v>
+      </c>
+      <c r="M38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.35392884331135493</v>
+      </c>
+      <c r="N38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.35392884331135493</v>
+      </c>
+      <c r="O38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.35392884331135493</v>
+      </c>
+      <c r="Q38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.66794647398026585</v>
+      </c>
+      <c r="R38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.8885245269079004</v>
+      </c>
+      <c r="S38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.66794647398026585</v>
+      </c>
+      <c r="U38" s="8">
+        <f>AVERAGE(A38,E38,I38,M38,Q38)</f>
+        <v>0.71581422734065803</v>
+      </c>
+      <c r="V38" s="8">
+        <f t="shared" ref="V38:W39" si="2">AVERAGE(B38,F38,J38,N38,R38)</f>
+        <v>0.77307060498150704</v>
+      </c>
+      <c r="W38" s="8">
+        <f t="shared" si="2"/>
+        <v>0.71728736646813007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <f>AVERAGE(A3,A6,A9,A12,A15,A18,A21,A24,A27,A30,A33,A36)</f>
+        <v>8.795916655799374E-4</v>
+      </c>
+      <c r="B39" s="6">
+        <f t="shared" si="0"/>
+        <v>5.4069250036263838E-3</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="0"/>
+        <v>5.4615500072638197E-3</v>
+      </c>
+      <c r="E39" s="6">
+        <f t="shared" si="1"/>
+        <v>3.4667916625039652E-3</v>
+      </c>
+      <c r="F39" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9182441673668411E-2</v>
+      </c>
+      <c r="G39" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6242508339928463E-2</v>
+      </c>
+      <c r="I39" s="6">
+        <f t="shared" si="1"/>
+        <v>5.2141250101461383E-3</v>
+      </c>
+      <c r="J39" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2408374997515541E-2</v>
+      </c>
+      <c r="K39" s="6">
+        <f t="shared" si="1"/>
+        <v>2.0924275008534703E-2</v>
+      </c>
+      <c r="M39" s="6">
+        <f t="shared" si="1"/>
+        <v>4.6623083471786231E-3</v>
+      </c>
+      <c r="N39" s="6">
+        <f t="shared" si="1"/>
+        <v>2.9911916664180655E-2</v>
+      </c>
+      <c r="O39" s="6">
+        <f t="shared" si="1"/>
+        <v>2.8285458334721625E-2</v>
+      </c>
+      <c r="Q39" s="6">
+        <f t="shared" si="1"/>
+        <v>3.293658335072299E-3</v>
+      </c>
+      <c r="R39" s="6">
+        <f t="shared" si="1"/>
+        <v>1.7064841672739323E-2</v>
+      </c>
+      <c r="S39" s="6">
+        <f t="shared" si="1"/>
+        <v>1.7203608343455318E-2</v>
+      </c>
+      <c r="U39" s="8">
+        <f>AVERAGE(A39,E39,I39,M39,Q39)</f>
+        <v>3.5032950040961922E-3</v>
+      </c>
+      <c r="V39" s="8">
+        <f t="shared" si="2"/>
+        <v>1.8794900002346064E-2</v>
+      </c>
+      <c r="W39" s="8">
+        <f t="shared" si="2"/>
+        <v>1.7623480006780788E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>